<commit_message>
Modify upper income limit
With a change in the translation function, the upper limit of income
needed to be increased
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +642,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>200000</v>
+        <v>270000</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>